<commit_message>
Added a main.py file to make it easier to tweak user inputs
</commit_message>
<xml_diff>
--- a/gw2_flip_volume_analysis.xlsx
+++ b/gw2_flip_volume_analysis.xlsx
@@ -694,16 +694,16 @@
         <v>24692</v>
       </c>
       <c r="C6" t="n">
-        <v>1460222</v>
+        <v>1460223</v>
       </c>
       <c r="D6" t="n">
         <v>1949999</v>
       </c>
       <c r="E6" t="n">
-        <v>19.72771499999999</v>
+        <v>19.72761499999999</v>
       </c>
       <c r="F6" t="n">
-        <v>13.51007928931354</v>
+        <v>13.51000155455707</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -816,23 +816,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ghostly Infusion</t>
+          <t>Vintage Black Lion Weapon Box</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>24207</v>
+        <v>26458</v>
       </c>
       <c r="C9" t="n">
-        <v>624998</v>
+        <v>400019</v>
       </c>
       <c r="D9" t="n">
-        <v>784994</v>
+        <v>523332</v>
       </c>
       <c r="E9" t="n">
-        <v>4.224690000000002</v>
+        <v>4.481320000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>6.759525630482022</v>
+        <v>11.20276786852625</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>29.382</v>
+        <v>103.885</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -859,23 +859,23 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Zojja''s Berserker Insignia</t>
+          <t>Ghostly Infusion</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>20887</v>
+        <v>24207</v>
       </c>
       <c r="C10" t="n">
-        <v>179140</v>
+        <v>624998</v>
       </c>
       <c r="D10" t="n">
-        <v>244495</v>
+        <v>784994</v>
       </c>
       <c r="E10" t="n">
-        <v>2.868075</v>
+        <v>4.224690000000002</v>
       </c>
       <c r="F10" t="n">
-        <v>16.01024338506196</v>
+        <v>6.759525630482022</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -886,13 +886,13 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>27.679</v>
+        <v>29.382</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -902,23 +902,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Polysaturating Reverberating Infusion (Purple)</t>
+          <t>Zojja''s Berserker Insignia</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25657</v>
+        <v>20887</v>
       </c>
       <c r="C11" t="n">
-        <v>330212</v>
+        <v>179140</v>
       </c>
       <c r="D11" t="n">
-        <v>419995</v>
+        <v>244480</v>
       </c>
       <c r="E11" t="n">
-        <v>2.678375</v>
+        <v>2.8668</v>
       </c>
       <c r="F11" t="n">
-        <v>8.111077126209828</v>
+        <v>16.00312604666741</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -929,16 +929,16 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>10.095</v>
+        <v>27.681</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9999999999999297</v>
+        <v>1</v>
       </c>
       <c r="M11" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Added a profit tracker to keep track of flips over time, ignores sells without matching buy orders and random sells below 10g as these are most likely not flips, as well as an ignore list for certain items that should be ignored regardless
</commit_message>
<xml_diff>
--- a/gw2_flip_volume_analysis.xlsx
+++ b/gw2_flip_volume_analysis.xlsx
@@ -510,59 +510,59 @@
         <v>24077</v>
       </c>
       <c r="C2" t="n">
-        <v>1750001</v>
+        <v>1900004</v>
       </c>
       <c r="D2" t="n">
-        <v>4300000</v>
+        <v>4349998</v>
       </c>
       <c r="E2" t="n">
-        <v>190.4999</v>
+        <v>179.74943</v>
       </c>
       <c r="F2" t="n">
-        <v>108.8570235102723</v>
+        <v>94.60476398997054</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>OK_LIQUID</t>
+          <t>OK_SLOW</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>0.478</v>
+        <v>0.323</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7615543404590253</v>
+        <v>0.6204853842040662</v>
       </c>
       <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Shrouded Bench of the Final Judge</t>
+          <t>Glyph of the Unbound (Unused)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25253</v>
+        <v>25441</v>
       </c>
       <c r="C3" t="n">
-        <v>1182110</v>
+        <v>2010002</v>
       </c>
       <c r="D3" t="n">
-        <v>2289882</v>
+        <v>2888483</v>
       </c>
       <c r="E3" t="n">
-        <v>76.42896999999999</v>
+        <v>44.52085499999998</v>
       </c>
       <c r="F3" t="n">
-        <v>64.65470218507583</v>
+        <v>22.14965706501783</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
@@ -595,36 +595,34 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Celestial Infusion (Blue)</t>
+          <t>Ignus Fatuus</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>24682</v>
+        <v>15717</v>
       </c>
       <c r="C4" t="n">
-        <v>1100001</v>
+        <v>2696969</v>
       </c>
       <c r="D4" t="n">
-        <v>1680784</v>
+        <v>3669998</v>
       </c>
       <c r="E4" t="n">
-        <v>32.86653999999999</v>
+        <v>42.25292999999998</v>
       </c>
       <c r="F4" t="n">
-        <v>29.87864556486766</v>
+        <v>15.66682079030199</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>NO_FLOW</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>OK_LIQUID</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -633,77 +631,73 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Trading observed, but effective daily sell-through rate collapsed to ~0 due to sparse or volatile recent activity</t>
-        </is>
-      </c>
+        <v>0.9396660624621362</v>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Crustacea</t>
+          <t>Fox Fire Spear Skin</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19937</v>
+        <v>332607</v>
       </c>
       <c r="C5" t="n">
-        <v>1400011</v>
+        <v>850010</v>
       </c>
       <c r="D5" t="n">
-        <v>1889896</v>
+        <v>1449897</v>
       </c>
       <c r="E5" t="n">
-        <v>20.64005999999999</v>
+        <v>38.24024499999999</v>
       </c>
       <c r="F5" t="n">
-        <v>14.7427841638387</v>
+        <v>44.98799425889107</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>OK_LIQUID</t>
+          <t>HOLD_RISK</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="I5" t="n">
-        <v>1.964</v>
+        <v>0.01</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9972409035899953</v>
+        <v>0.03036139133931093</v>
       </c>
       <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Advanced Leather Rack</t>
+          <t>Arthropoda</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24692</v>
+        <v>19936</v>
       </c>
       <c r="C6" t="n">
-        <v>1460223</v>
+        <v>965729</v>
       </c>
       <c r="D6" t="n">
-        <v>1949999</v>
+        <v>1366670</v>
       </c>
       <c r="E6" t="n">
-        <v>19.72761499999999</v>
+        <v>19.59405</v>
       </c>
       <c r="F6" t="n">
-        <v>13.51000155455707</v>
+        <v>20.28938760252617</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -714,39 +708,39 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>2.311</v>
+        <v>1.097</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>0.999026222939765</v>
+        <v>0.9627948221649534</v>
       </c>
       <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dragon''s Claw</t>
+          <t>Winter''s Heart Infusion</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>26559</v>
+        <v>24511</v>
       </c>
       <c r="C7" t="n">
-        <v>1214803</v>
+        <v>1657076</v>
       </c>
       <c r="D7" t="n">
-        <v>1556660</v>
+        <v>2149999</v>
       </c>
       <c r="E7" t="n">
-        <v>10.8358</v>
+        <v>17.04231499999999</v>
       </c>
       <c r="F7" t="n">
-        <v>8.919800165129654</v>
+        <v>10.28457053267321</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -757,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>2.028</v>
+        <v>2.385</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -766,30 +760,30 @@
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9977199825885696</v>
+        <v>0.9992193330446831</v>
       </c>
       <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Collapsing Star Spear Skin</t>
+          <t>+14 Agony Infusion</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>693816</v>
+        <v>21827</v>
       </c>
       <c r="C8" t="n">
-        <v>837385</v>
+        <v>1510004</v>
       </c>
       <c r="D8" t="n">
-        <v>1050000</v>
+        <v>1899999</v>
       </c>
       <c r="E8" t="n">
-        <v>5.5115</v>
+        <v>10.49951499999999</v>
       </c>
       <c r="F8" t="n">
-        <v>6.581799291843058</v>
+        <v>6.953302772707881</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -800,39 +794,39 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1.762</v>
+        <v>2.106</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9949364845589463</v>
+        <v>0.9981970142173253</v>
       </c>
       <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vintage Black Lion Weapon Box</t>
+          <t>Elder Wood Logging Node</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>26458</v>
+        <v>22586</v>
       </c>
       <c r="C9" t="n">
-        <v>400019</v>
+        <v>1000003</v>
       </c>
       <c r="D9" t="n">
-        <v>523332</v>
+        <v>1299750</v>
       </c>
       <c r="E9" t="n">
-        <v>4.481320000000001</v>
+        <v>10.47845</v>
       </c>
       <c r="F9" t="n">
-        <v>11.20276786852625</v>
+        <v>10.47841856474431</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -840,10 +834,10 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>103.885</v>
+        <v>0.733</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -852,7 +846,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>0.889031248563259</v>
       </c>
       <c r="M9" t="inlineStr"/>
     </row>
@@ -863,19 +857,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24207</v>
+        <v>24213</v>
       </c>
       <c r="C10" t="n">
-        <v>624998</v>
+        <v>609994</v>
       </c>
       <c r="D10" t="n">
-        <v>784994</v>
+        <v>839990</v>
       </c>
       <c r="E10" t="n">
-        <v>4.224690000000002</v>
+        <v>10.39975</v>
       </c>
       <c r="F10" t="n">
-        <v>6.759525630482022</v>
+        <v>17.04893818627724</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -886,39 +880,39 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>29.382</v>
+        <v>8.676</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0.9999999999950331</v>
       </c>
       <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zojja''s Berserker Insignia</t>
+          <t>Winter''s Heart Infusion</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>20887</v>
+        <v>24517</v>
       </c>
       <c r="C11" t="n">
-        <v>179140</v>
+        <v>880725</v>
       </c>
       <c r="D11" t="n">
-        <v>244480</v>
+        <v>1158090</v>
       </c>
       <c r="E11" t="n">
-        <v>2.8668</v>
+        <v>10.36515</v>
       </c>
       <c r="F11" t="n">
-        <v>16.00312604666741</v>
+        <v>11.76888359022396</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -929,16 +923,16 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>27.681</v>
+        <v>2.965</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>0.9998629051024138</v>
       </c>
       <c r="M11" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Sorting initial item list by roi to show high value investments first
</commit_message>
<xml_diff>
--- a/gw2_flip_volume_analysis.xlsx
+++ b/gw2_flip_volume_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,76 +503,80 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Essence of Ebonhawke</t>
+          <t>Shadow Chevalier Torch Skin</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24077</v>
+        <v>27416</v>
       </c>
       <c r="C2" t="n">
-        <v>1900004</v>
+        <v>868790</v>
       </c>
       <c r="D2" t="n">
-        <v>4349998</v>
+        <v>4000000</v>
       </c>
       <c r="E2" t="n">
-        <v>179.74943</v>
+        <v>253.121</v>
       </c>
       <c r="F2" t="n">
-        <v>94.60476398997054</v>
+        <v>291.3488875332359</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>OK_SLOW</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="I2" t="n">
-        <v>0.323</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6204853842040662</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>6 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Glyph of the Unbound (Unused)</t>
+          <t>Winter''s Heart Infusion</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25441</v>
+        <v>24511</v>
       </c>
       <c r="C3" t="n">
-        <v>2010002</v>
+        <v>1200349</v>
       </c>
       <c r="D3" t="n">
-        <v>2888483</v>
+        <v>1985002</v>
       </c>
       <c r="E3" t="n">
-        <v>44.52085499999998</v>
+        <v>48.69027</v>
       </c>
       <c r="F3" t="n">
-        <v>22.14965706501783</v>
+        <v>40.5634278030806</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>NO_FLOW</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>HOLD_RISK</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3970004</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -581,166 +585,174 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Trading observed, but effective daily sell-through rate collapsed to ~0 due to sparse or volatile recent activity</t>
-        </is>
-      </c>
+        <v>7.55666459406612e-07</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ignus Fatuus</t>
+          <t>Crustacea</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15717</v>
+        <v>19937</v>
       </c>
       <c r="C4" t="n">
-        <v>2696969</v>
+        <v>1350000</v>
       </c>
       <c r="D4" t="n">
-        <v>3669998</v>
+        <v>1890000</v>
       </c>
       <c r="E4" t="n">
-        <v>42.25292999999998</v>
+        <v>25.65</v>
       </c>
       <c r="F4" t="n">
-        <v>15.66682079030199</v>
+        <v>19</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>OK_LIQUID</t>
+          <t>OK_SLOW</t>
         </is>
       </c>
       <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.9360000000000001</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
       <c r="L4" t="n">
-        <v>0.9396660624621362</v>
+        <v>0.505852993582407</v>
       </c>
       <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fox Fire Spear Skin</t>
+          <t>Polysaturating Reverberating Infusion (Gray)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>332607</v>
+        <v>25627</v>
       </c>
       <c r="C5" t="n">
-        <v>850010</v>
+        <v>1470530</v>
       </c>
       <c r="D5" t="n">
-        <v>1449897</v>
+        <v>1989893</v>
       </c>
       <c r="E5" t="n">
-        <v>38.24024499999999</v>
+        <v>22.08790500000001</v>
       </c>
       <c r="F5" t="n">
-        <v>44.98799425889107</v>
+        <v>15.02037020666019</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>HOLD_RISK</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>98</v>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="I5" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L5" t="n">
-        <v>0.03036139133931093</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>4 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Arthropoda</t>
+          <t>Phospholuminescent Infusion</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>19936</v>
+        <v>24480</v>
       </c>
       <c r="C6" t="n">
-        <v>965729</v>
+        <v>1390711</v>
       </c>
       <c r="D6" t="n">
-        <v>1366670</v>
+        <v>1849999</v>
       </c>
       <c r="E6" t="n">
-        <v>19.59405</v>
+        <v>18.17881499999999</v>
       </c>
       <c r="F6" t="n">
-        <v>20.28938760252617</v>
+        <v>13.07159790927086</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>OK_LIQUID</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="I6" t="n">
-        <v>1.097</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9627948221649534</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>3 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Winter''s Heart Infusion</t>
+          <t>Peerless Infusion</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>24511</v>
+        <v>25865</v>
       </c>
       <c r="C7" t="n">
-        <v>1657076</v>
+        <v>1027081</v>
       </c>
       <c r="D7" t="n">
-        <v>2149999</v>
+        <v>1349992</v>
       </c>
       <c r="E7" t="n">
-        <v>17.04231499999999</v>
+        <v>12.04122</v>
       </c>
       <c r="F7" t="n">
-        <v>10.28457053267321</v>
+        <v>11.72372967662725</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -748,42 +760,42 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>2.385</v>
+        <v>0.544</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9992193330446831</v>
+        <v>0.804581071730771</v>
       </c>
       <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>+14 Agony Infusion</t>
+          <t>Winter''s Heart Infusion</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>21827</v>
+        <v>24517</v>
       </c>
       <c r="C8" t="n">
-        <v>1510004</v>
+        <v>955004</v>
       </c>
       <c r="D8" t="n">
-        <v>1899999</v>
+        <v>1199999</v>
       </c>
       <c r="E8" t="n">
-        <v>10.49951499999999</v>
+        <v>6.499515000000002</v>
       </c>
       <c r="F8" t="n">
-        <v>6.953302772707881</v>
+        <v>6.805746363366019</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -791,42 +803,42 @@
         </is>
       </c>
       <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="I8" t="n">
-        <v>2.106</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
       <c r="L8" t="n">
-        <v>0.9981970142173253</v>
+        <v>0.8905749669380867</v>
       </c>
       <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Elder Wood Logging Node</t>
+          <t>Ghostly Infusion</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>22586</v>
+        <v>24206</v>
       </c>
       <c r="C9" t="n">
-        <v>1000003</v>
+        <v>523241</v>
       </c>
       <c r="D9" t="n">
-        <v>1299750</v>
+        <v>679907</v>
       </c>
       <c r="E9" t="n">
-        <v>10.47845</v>
+        <v>5.467994999999996</v>
       </c>
       <c r="F9" t="n">
-        <v>10.47841856474431</v>
+        <v>10.45024185795837</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -834,19 +846,19 @@
         </is>
       </c>
       <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
         <v>2</v>
       </c>
-      <c r="I9" t="n">
-        <v>0.733</v>
-      </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
       <c r="L9" t="n">
-        <v>0.889031248563259</v>
+        <v>0.7750489414166475</v>
       </c>
       <c r="M9" t="inlineStr"/>
     </row>
@@ -857,84 +869,323 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24213</v>
+        <v>24216</v>
       </c>
       <c r="C10" t="n">
-        <v>609994</v>
+        <v>518379</v>
       </c>
       <c r="D10" t="n">
-        <v>839990</v>
+        <v>669889</v>
       </c>
       <c r="E10" t="n">
-        <v>10.39975</v>
+        <v>5.102665000000003</v>
       </c>
       <c r="F10" t="n">
-        <v>17.04893818627724</v>
+        <v>9.843502533860365</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>OK_LIQUID</t>
+          <t>HOLD_RISK</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="I10" t="n">
-        <v>8.676</v>
+        <v>0.003</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9999999999950331</v>
+        <v>0.008204093178705296</v>
       </c>
       <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Winter''s Heart Infusion</t>
+          <t>Ghostly Infusion</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>24517</v>
+        <v>24207</v>
       </c>
       <c r="C11" t="n">
-        <v>880725</v>
+        <v>640010</v>
       </c>
       <c r="D11" t="n">
-        <v>1158090</v>
+        <v>779791</v>
       </c>
       <c r="E11" t="n">
-        <v>10.36515</v>
+        <v>2.281234999999997</v>
       </c>
       <c r="F11" t="n">
-        <v>11.76888359022396</v>
+        <v>3.564373994156337</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>NO_FLOW</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Trading observed, but effective daily sell-through rate collapsed to ~0 due to sparse or volatile recent activity</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Zojja''s Berserker Insignia</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>20887</v>
+      </c>
+      <c r="C12" t="n">
+        <v>205601</v>
+      </c>
+      <c r="D12" t="n">
+        <v>260000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.5399</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.489749563474886</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>OK_LIQUID</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H12" t="n">
         <v>1</v>
       </c>
-      <c r="I11" t="n">
-        <v>2.965</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="I12" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
         <v>1</v>
       </c>
-      <c r="L11" t="n">
-        <v>0.9998629051024138</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Zojja''s Berserker Inscription</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>20865</v>
+      </c>
+      <c r="C13" t="n">
+        <v>250543</v>
+      </c>
+      <c r="D13" t="n">
+        <v>309543</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.256854999999999</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5.01652410963387</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>3 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Vintage Black Lion Weapon Box</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>26458</v>
+      </c>
+      <c r="C14" t="n">
+        <v>420001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>508725</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.241525</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.956004866655079</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>3 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jade Bot Core: Tier 10</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>26651</v>
+      </c>
+      <c r="C15" t="n">
+        <v>447630</v>
+      </c>
+      <c r="D15" t="n">
+        <v>472000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-4.643</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-10.37240578156066</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>OK_LIQUID</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>31.375</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mystic Facet</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>27392</v>
+      </c>
+      <c r="C16" t="n">
+        <v>725017</v>
+      </c>
+      <c r="D16" t="n">
+        <v>794999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-4.926784999999998</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-6.79540617668275</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>DEADLIKE</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>4 consecutive zero-unit days in last 7</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>